<commit_message>
Updated code part 2 - generating random email id
</commit_message>
<xml_diff>
--- a/src/test/resources/registration.xlsx
+++ b/src/test/resources/registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suponugupati\IdeaProjects\OpenMRS\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167751E7-FA90-475C-83B5-1A1267E8E25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF0DEF8-FE03-40DD-B8FD-B81DD8E8168E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>data01</t>
   </si>
   <si>
-    <t>data02</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -45,127 +42,19 @@
     <t>Password</t>
   </si>
   <si>
-    <t>User 1</t>
-  </si>
-  <si>
     <t>ABCD@123</t>
   </si>
   <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>User 2</t>
-  </si>
-  <si>
-    <t>testuser2@gmail.com</t>
-  </si>
-  <si>
-    <t>ABCDEF@123</t>
-  </si>
-  <si>
     <t>test data</t>
   </si>
   <si>
-    <t>Test 111</t>
-  </si>
-  <si>
-    <t>testuser111@gmail.com</t>
-  </si>
-  <si>
-    <t>data03</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>User 3</t>
-  </si>
-  <si>
-    <t>data04</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>Test 6</t>
-  </si>
-  <si>
-    <t>Test 7</t>
-  </si>
-  <si>
-    <t>Test 8</t>
-  </si>
-  <si>
-    <t>Test 9</t>
-  </si>
-  <si>
-    <t>Test 10</t>
-  </si>
-  <si>
-    <t>User 4</t>
-  </si>
-  <si>
-    <t>User 5</t>
-  </si>
-  <si>
-    <t>User 6</t>
-  </si>
-  <si>
-    <t>User 7</t>
-  </si>
-  <si>
-    <t>User 8</t>
-  </si>
-  <si>
-    <t>User 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User 10 </t>
-  </si>
-  <si>
-    <t>data10</t>
-  </si>
-  <si>
-    <t>data9</t>
-  </si>
-  <si>
-    <t>data8</t>
-  </si>
-  <si>
-    <t>data7</t>
-  </si>
-  <si>
-    <t>data6</t>
-  </si>
-  <si>
-    <t>data5</t>
-  </si>
-  <si>
-    <t>testuser3@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser4@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser5@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser6@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser7@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser8@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser9@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser10@gmail.com</t>
+    <t>testuser@gmail.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>User</t>
   </si>
 </sst>
 </file>
@@ -505,7 +394,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,19 +407,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -538,195 +427,84 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{3C26B9F7-1D92-4673-B186-BBEA0B93FB32}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{CF066CAB-1254-42D0-90F0-30E023013D14}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{19FA5E1E-EA1E-4544-88F9-93F02C7ADAC8}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{7FA9FC3A-9DEE-43BA-8752-DBA79ED66645}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{FEBCF2A1-840C-4AB2-AD07-13EAC8BD93B0}"/>
-    <hyperlink ref="E4" r:id="rId6" xr:uid="{B10CCBAE-5701-416E-9553-014AA28923E2}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{7D63C7BF-E63C-454C-9E0C-4515304B4A91}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{4858E119-EC44-4801-84EA-0309B56E59A4}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{33D3A8FE-5E63-4D2E-AEF2-E5E1DCF57BCC}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{5C4DFC42-1910-443A-8DD1-1679108AC9B5}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{07794FF6-B003-466A-B16F-88485620263E}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{EFF548FC-F38D-4DEE-B4C9-04EB897C1DDA}"/>
-    <hyperlink ref="D8" r:id="rId13" xr:uid="{AD489BF9-C5D3-4022-8AA8-BCA52438CFED}"/>
-    <hyperlink ref="E8" r:id="rId14" xr:uid="{A4AF39F2-F394-49DE-8CCD-B157739D0029}"/>
-    <hyperlink ref="D9" r:id="rId15" xr:uid="{38AE03DE-6330-4805-A5D1-80F3FBA1437A}"/>
-    <hyperlink ref="E9" r:id="rId16" xr:uid="{67ECA710-C80D-4F5B-9EA3-9F17BEC2987F}"/>
-    <hyperlink ref="D10" r:id="rId17" xr:uid="{F8EF744F-3ACB-4952-B460-EB036DAC78E5}"/>
-    <hyperlink ref="E10" r:id="rId18" xr:uid="{4E3B6AB1-60C1-4C9E-8ABB-AAB8336204D9}"/>
-    <hyperlink ref="D11" r:id="rId19" xr:uid="{B1455D29-4CC0-43E5-B4AC-ADFCCB14E4A7}"/>
-    <hyperlink ref="E11" r:id="rId20" xr:uid="{D4547EA0-AFB7-4AB9-8811-2E8CBD438FAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>